<commit_message>
removed unwanted code for extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/UsersAPI.xlsx
+++ b/src/test/resources/exceldata/UsersAPI.xlsx
@@ -917,9 +917,7 @@
       <c r="K2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="s">
-        <v>60</v>
-      </c>
+      <c r="L2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -952,9 +950,7 @@
       <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="L3" t="s">
-        <v>61</v>
-      </c>
+      <c r="L3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">

</xml_diff>